<commit_message>
Forage Box forms for on-farm, ce1 and ce2
V1 for CE1 and CE2
V1 for on-farm, first since split from the beta test. Includes walking media files, and places to describe the walking patterns for CE1 and CE2.
</commit_message>
<xml_diff>
--- a/forms/psa_corn_disease/psa_corn_disease.xlsx
+++ b/forms/psa_corn_disease/psa_corn_disease.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="227">
   <si>
     <t>type</t>
   </si>
@@ -702,7 +702,7 @@
     <t>weightnote</t>
   </si>
   <si>
-    <t>Places to take dry weights will appear in this form here if any of your reps required sampling. Fill in any that are applicable and leave others blank.  If you were not prompted to dig plants, you can finish and submit the form.</t>
+    <t>Take dry weights of any plants that  required sampling. Fill in any that are applicable and leave others blank.  If you were not prompted to dig plants, you can finish and submit the form.</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1047,7 @@
   <dimension ref="A1:I119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+      <selection activeCell="I111" sqref="I111:I118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2583,9 +2583,6 @@
       <c r="D111" t="s">
         <v>15</v>
       </c>
-      <c r="I111" t="s">
-        <v>167</v>
-      </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
@@ -2600,11 +2597,8 @@
       <c r="D112" t="s">
         <v>15</v>
       </c>
-      <c r="I112" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>193</v>
       </c>
@@ -2617,11 +2611,8 @@
       <c r="D113" t="s">
         <v>15</v>
       </c>
-      <c r="I113" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>193</v>
       </c>
@@ -2634,11 +2625,8 @@
       <c r="D114" t="s">
         <v>15</v>
       </c>
-      <c r="I114" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>193</v>
       </c>
@@ -2651,11 +2639,8 @@
       <c r="D115" t="s">
         <v>15</v>
       </c>
-      <c r="I115" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>193</v>
       </c>
@@ -2668,11 +2653,8 @@
       <c r="D116" t="s">
         <v>15</v>
       </c>
-      <c r="I116" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>193</v>
       </c>
@@ -2685,11 +2667,8 @@
       <c r="D117" t="s">
         <v>15</v>
       </c>
-      <c r="I117" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>193</v>
       </c>
@@ -2702,11 +2681,8 @@
       <c r="D118" t="s">
         <v>15</v>
       </c>
-      <c r="I118" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>38</v>
       </c>

</xml_diff>